<commit_message>
Created Slot.cs Updated sheet
</commit_message>
<xml_diff>
--- a/DotNet_Project.xlsx
+++ b/DotNet_Project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533491\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533622\Documents\44663\DotnetProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -348,10 +348,10 @@
     <t>NumberOFTerms(U, 5)</t>
   </si>
   <si>
-    <t>DegreePlan (FK)</t>
+    <t>B</t>
   </si>
   <si>
-    <t>B</t>
+    <t>DegreePlanID (FK)</t>
   </si>
 </sst>
 </file>
@@ -7496,7 +7496,7 @@
         <v>356</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="12"/>
     </row>
@@ -7514,7 +7514,7 @@
         <v>542</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F3" s="12"/>
     </row>
@@ -7568,7 +7568,7 @@
         <v>664</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -7586,7 +7586,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" s="12"/>
     </row>
@@ -7604,7 +7604,7 @@
         <v>618</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -7622,7 +7622,7 @@
         <v>691</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="12"/>
     </row>
@@ -7640,7 +7640,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" s="12"/>
     </row>
@@ -7658,7 +7658,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" s="12"/>
     </row>
@@ -7676,7 +7676,7 @@
         <v>692</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="12"/>
     </row>
@@ -7694,7 +7694,7 @@
         <v>555</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" s="12"/>
     </row>
@@ -7712,7 +7712,7 @@
         <v>356</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -7730,7 +7730,7 @@
         <v>542</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" s="12"/>
     </row>
@@ -7748,7 +7748,7 @@
         <v>563</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -7766,7 +7766,7 @@
         <v>560</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -7784,7 +7784,7 @@
         <v>664</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="12"/>
     </row>
@@ -7802,7 +7802,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -7820,7 +7820,7 @@
         <v>618</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F20" s="12"/>
     </row>
@@ -7838,7 +7838,7 @@
         <v>691</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" s="12"/>
     </row>
@@ -7856,7 +7856,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" s="12"/>
     </row>
@@ -7874,7 +7874,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F23" s="12"/>
     </row>
@@ -7892,7 +7892,7 @@
         <v>692</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" s="12"/>
     </row>
@@ -7910,7 +7910,7 @@
         <v>555</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F25" s="12"/>
     </row>
@@ -7928,7 +7928,7 @@
         <v>356</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" s="12"/>
     </row>
@@ -7946,7 +7946,7 @@
         <v>542</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="12"/>
     </row>
@@ -9299,7 +9299,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9317,7 +9317,7 @@
         <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
ADDED DATA in slot table
</commit_message>
<xml_diff>
--- a/DotNet_Project.xlsx
+++ b/DotNet_Project.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533727\Documents\44-663\DotnetProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\S533705\44663\DotnetProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="110">
   <si>
     <t>CreditID(PK)</t>
   </si>
@@ -356,6 +356,9 @@
   <si>
     <t>As fast as I can</t>
   </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
@@ -445,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -492,11 +495,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -612,6 +624,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1969,7 +1984,7 @@
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4744,8 +4759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7511,10 +7526,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1001"/>
+  <dimension ref="A1:G1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8807,49 +8822,435 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A74" s="42"/>
-      <c r="B74" s="42"/>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="98" spans="7:7" ht="15.75" customHeight="1">
-      <c r="G98" s="19"/>
-    </row>
-    <row r="99" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="100" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="101" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="102" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="103" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="104" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="105" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="106" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="107" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="108" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="109" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="110" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="111" spans="7:7" ht="15.75" customHeight="1"/>
-    <row r="112" spans="7:7" ht="15.75" customHeight="1"/>
+      <c r="A74" s="16">
+        <v>74</v>
+      </c>
+      <c r="B74" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C74" s="42">
+        <v>1</v>
+      </c>
+      <c r="D74" s="42">
+        <v>542</v>
+      </c>
+      <c r="E74" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A75" s="16">
+        <v>75</v>
+      </c>
+      <c r="B75" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C75" s="42">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>356</v>
+      </c>
+      <c r="E75" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A76" s="16">
+        <v>76</v>
+      </c>
+      <c r="B76" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C76" s="42">
+        <v>1</v>
+      </c>
+      <c r="D76" s="42">
+        <v>563</v>
+      </c>
+      <c r="E76" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A77" s="16">
+        <v>77</v>
+      </c>
+      <c r="B77" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C77" s="42">
+        <v>2</v>
+      </c>
+      <c r="D77" s="42">
+        <v>560</v>
+      </c>
+      <c r="E77" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A78" s="16">
+        <v>78</v>
+      </c>
+      <c r="B78" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C78" s="42">
+        <v>2</v>
+      </c>
+      <c r="D78" s="42">
+        <v>6</v>
+      </c>
+      <c r="E78" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A79" s="16">
+        <v>79</v>
+      </c>
+      <c r="B79" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C79" s="42">
+        <v>2</v>
+      </c>
+      <c r="D79" s="42">
+        <v>555</v>
+      </c>
+      <c r="E79" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A80" s="16">
+        <v>80</v>
+      </c>
+      <c r="B80" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C80" s="42">
+        <v>3</v>
+      </c>
+      <c r="D80" s="42">
+        <v>664</v>
+      </c>
+      <c r="E80" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A81" s="16">
+        <v>81</v>
+      </c>
+      <c r="B81" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C81" s="42">
+        <v>3</v>
+      </c>
+      <c r="D81" s="42">
+        <v>691</v>
+      </c>
+      <c r="E81" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A82" s="16">
+        <v>82</v>
+      </c>
+      <c r="B82" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C82" s="42">
+        <v>3</v>
+      </c>
+      <c r="D82" s="42">
+        <v>618</v>
+      </c>
+      <c r="E82" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A83" s="16">
+        <v>83</v>
+      </c>
+      <c r="B83" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C83" s="42">
+        <v>4</v>
+      </c>
+      <c r="D83" s="42">
+        <v>692</v>
+      </c>
+      <c r="E83" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A84" s="16">
+        <v>84</v>
+      </c>
+      <c r="B84" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C84" s="42">
+        <v>4</v>
+      </c>
+      <c r="D84" s="42">
+        <v>10</v>
+      </c>
+      <c r="E84" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A85" s="16">
+        <v>85</v>
+      </c>
+      <c r="B85" s="42">
+        <v>7253</v>
+      </c>
+      <c r="C85" s="42">
+        <v>4</v>
+      </c>
+      <c r="D85" s="42">
+        <v>20</v>
+      </c>
+      <c r="E85" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A86" s="16">
+        <v>86</v>
+      </c>
+      <c r="B86" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C86" s="42">
+        <v>1</v>
+      </c>
+      <c r="D86" s="42">
+        <v>356</v>
+      </c>
+      <c r="E86" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A87" s="16">
+        <v>87</v>
+      </c>
+      <c r="B87" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C87" s="42">
+        <v>1</v>
+      </c>
+      <c r="D87" s="42">
+        <v>542</v>
+      </c>
+      <c r="E87" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A88" s="16">
+        <v>88</v>
+      </c>
+      <c r="B88" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C88" s="42">
+        <v>1</v>
+      </c>
+      <c r="D88" s="42">
+        <v>563</v>
+      </c>
+      <c r="E88" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A89" s="16">
+        <v>89</v>
+      </c>
+      <c r="B89" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C89" s="42">
+        <v>2</v>
+      </c>
+      <c r="D89" s="42">
+        <v>560</v>
+      </c>
+      <c r="E89" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A90" s="16">
+        <v>90</v>
+      </c>
+      <c r="B90" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C90" s="42">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <v>664</v>
+      </c>
+      <c r="E90" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A91" s="16">
+        <v>91</v>
+      </c>
+      <c r="B91" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C91" s="42">
+        <v>2</v>
+      </c>
+      <c r="D91" s="42">
+        <v>6</v>
+      </c>
+      <c r="E91" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A92" s="16">
+        <v>92</v>
+      </c>
+      <c r="B92" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C92" s="42">
+        <v>3</v>
+      </c>
+      <c r="D92" s="42">
+        <v>691</v>
+      </c>
+      <c r="E92" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A93" s="16">
+        <v>93</v>
+      </c>
+      <c r="B93" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C93" s="42">
+        <v>3</v>
+      </c>
+      <c r="D93" s="42">
+        <v>10</v>
+      </c>
+      <c r="E93" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A94" s="16">
+        <v>94</v>
+      </c>
+      <c r="B94" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C94" s="42">
+        <v>3</v>
+      </c>
+      <c r="D94" s="42">
+        <v>20</v>
+      </c>
+      <c r="E94" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A95" s="16">
+        <v>95</v>
+      </c>
+      <c r="B95" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C95" s="42">
+        <v>4</v>
+      </c>
+      <c r="D95" s="42">
+        <v>618</v>
+      </c>
+      <c r="E95" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A96" s="16">
+        <v>96</v>
+      </c>
+      <c r="B96" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C96" s="42">
+        <v>5</v>
+      </c>
+      <c r="D96" s="43">
+        <v>692</v>
+      </c>
+      <c r="E96" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A97" s="16">
+        <v>97</v>
+      </c>
+      <c r="B97" s="42">
+        <v>7254</v>
+      </c>
+      <c r="C97" s="42">
+        <v>5</v>
+      </c>
+      <c r="D97" s="43">
+        <v>555</v>
+      </c>
+      <c r="E97" s="42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A98" s="16"/>
+      <c r="B98" s="42"/>
+    </row>
+    <row r="99" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A99" s="16"/>
+      <c r="B99" s="42"/>
+      <c r="G99" s="19"/>
+    </row>
+    <row r="100" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="101" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="102" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="103" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="104" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="105" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="106" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="107" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="108" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="109" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="110" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="111" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="112" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>
     <row r="115" ht="15.75" customHeight="1"/>
@@ -9739,6 +10140,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Excel sheet and Updated DbInitializer.cs
</commit_message>
<xml_diff>
--- a/DotNet_Project.xlsx
+++ b/DotNet_Project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533727\Documents\44-663\DotnetProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533622\Documents\44663\DotnetProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="110">
   <si>
     <t>CreditID(PK)</t>
   </si>
@@ -216,16 +216,7 @@
     <t>Himabindu</t>
   </si>
   <si>
-    <t>SlotID (PK)</t>
-  </si>
-  <si>
-    <t>DegreePlan(FK)</t>
-  </si>
-  <si>
     <t>Term</t>
-  </si>
-  <si>
-    <t>Status char(1)</t>
   </si>
   <si>
     <t>C</t>
@@ -351,13 +342,22 @@
     <t>DegreePlanID (FK)</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>As fast as I can</t>
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>DegreePlanID</t>
+  </si>
+  <si>
+    <t>CreditID</t>
+  </si>
+  <si>
+    <t>SlotID</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -495,11 +495,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -602,9 +615,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -618,6 +628,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,16 +943,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4746,10 +4775,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F998"/>
+  <dimension ref="A1:E998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4762,7 +4791,7 @@
     <col min="6" max="6" width="159.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -4775,14 +4804,11 @@
       <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="15">
         <v>7253</v>
       </c>
@@ -4793,17 +4819,13 @@
         <v>48</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="26">
+        <v>104</v>
+      </c>
+      <c r="E2" s="45">
         <v>3</v>
       </c>
-      <c r="F2" s="26" t="str">
-        <f>" DegreePlan{"&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;B2&amp;" ,"&amp;$C$1&amp;" ="&amp;C2&amp;" ,"&amp;$D$1&amp;" ="&amp;D2&amp;" ,"&amp;$E$1&amp;"="&amp;E2&amp;"}"</f>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7253 , StudentID (u, 10)(FK) = 533705 ,DegreePlanAbbrev(u,20) =Super fast ,DegreePlanName(u, 20) =As fast as I can ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="15">
         <v>7254</v>
       </c>
@@ -4816,15 +4838,11 @@
       <c r="D3" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="45">
         <v>3</v>
       </c>
-      <c r="F3" s="26" t="str">
-        <f t="shared" ref="F3:F11" si="0">" DegreePlan{"&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;B3&amp;" ,"&amp;$C$1&amp;" ="&amp;C3&amp;" ,"&amp;$D$1&amp;" ="&amp;D3&amp;" ,"&amp;$E$1&amp;"="&amp;E3&amp;"}"</f>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7254 , StudentID (u, 10)(FK) = 533705 ,DegreePlanAbbrev(u,20) =slow And Easy ,DegreePlanName(u, 20) =Take a summer Off ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="14">
         <v>7255</v>
       </c>
@@ -4834,18 +4852,14 @@
       <c r="C4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="25">
+      <c r="D4" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="46">
         <v>3</v>
       </c>
-      <c r="F4" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7255 , StudentID (u, 10)(FK) = 533491 ,DegreePlanAbbrev(u,20) =Super fast ,DegreePlanName(u, 20) =As fast as I can ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="14">
         <v>7256</v>
       </c>
@@ -4858,15 +4872,11 @@
       <c r="D5" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="46">
         <v>3</v>
       </c>
-      <c r="F5" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7256 , StudentID (u, 10)(FK) = 533491 ,DegreePlanAbbrev(u,20) =slow And Easy ,DegreePlanName(u, 20) =Take a summer Off ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="19">
         <v>7257</v>
       </c>
@@ -4876,18 +4886,14 @@
       <c r="C6" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="27">
+      <c r="D6" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="47">
         <v>3</v>
       </c>
-      <c r="F6" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7257 , StudentID (u, 10)(FK) = 533727 ,DegreePlanAbbrev(u,20) =SuperFast ,DegreePlanName(u, 20) =As fast as I can ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="19">
         <v>7258</v>
       </c>
@@ -4900,15 +4906,11 @@
       <c r="D7" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="47">
         <v>3</v>
       </c>
-      <c r="F7" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7258 , StudentID (u, 10)(FK) = 533727 ,DegreePlanAbbrev(u,20) =slow And Easy ,DegreePlanName(u, 20) =Take a summer Off ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="17">
         <v>7259</v>
       </c>
@@ -4921,15 +4923,11 @@
       <c r="D8" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="48">
         <v>3</v>
       </c>
-      <c r="F8" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7259 , StudentID (u, 10)(FK) = 533622 ,DegreePlanAbbrev(u,20) =slow And Easy ,DegreePlanName(u, 20) =Take a summer Off ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="17">
         <v>7260</v>
       </c>
@@ -4942,15 +4940,11 @@
       <c r="D9" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="48">
         <v>3</v>
       </c>
-      <c r="F9" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7260 , StudentID (u, 10)(FK) = 533622 ,DegreePlanAbbrev(u,20) =slow And Easy ,DegreePlanName(u, 20) =Take a summer Off ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="16">
         <v>7261</v>
       </c>
@@ -4960,18 +4954,14 @@
       <c r="C10" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="29">
+      <c r="D10" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="49">
         <v>3</v>
       </c>
-      <c r="F10" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7261 , StudentID (u, 10)(FK) = 533988 ,DegreePlanAbbrev(u,20) =Super fast ,DegreePlanName(u, 20) =As fast as I can ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="16">
         <v>7262</v>
       </c>
@@ -4984,18 +4974,14 @@
       <c r="D11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="49">
         <v>3</v>
       </c>
-      <c r="F11" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> DegreePlan{DegreePlanID(PK) = 7262 , StudentID (u, 10)(FK) = 533988 ,DegreePlanAbbrev(u,20) =slow And Easy ,DegreePlanName(u, 20) =Take a summer Off ,DegreeID (FK)=3}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
       <c r="D12" s="36"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="C13" s="9"/>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -7517,8 +7503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7528,25 +7514,25 @@
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="112.42578125" customWidth="1"/>
     <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="F1" s="12"/>
     </row>
@@ -7564,9 +7550,9 @@
         <v>356</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="14">
@@ -7582,9 +7568,9 @@
         <v>542</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="14">
@@ -7600,9 +7586,9 @@
         <v>563</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="14">
@@ -7618,9 +7604,9 @@
         <v>560</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="F5" s="43"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="14">
@@ -7636,9 +7622,9 @@
         <v>664</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F6" s="43"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="14">
@@ -7654,9 +7640,9 @@
         <v>6</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="14">
@@ -7672,9 +7658,9 @@
         <v>618</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="14">
@@ -7690,9 +7676,9 @@
         <v>691</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="14">
@@ -7708,9 +7694,9 @@
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F10" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="14">
@@ -7726,9 +7712,9 @@
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F11" s="43"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="14">
@@ -7744,9 +7730,9 @@
         <v>692</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="14">
@@ -7762,9 +7748,9 @@
         <v>555</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="14">
@@ -7780,9 +7766,9 @@
         <v>356</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="14">
@@ -7798,9 +7784,9 @@
         <v>542</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="14">
@@ -7816,9 +7802,9 @@
         <v>563</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="14">
@@ -7834,9 +7820,9 @@
         <v>560</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="14">
@@ -7852,9 +7838,9 @@
         <v>664</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="14">
@@ -7870,9 +7856,9 @@
         <v>6</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="14">
@@ -7888,9 +7874,9 @@
         <v>618</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="14">
@@ -7906,9 +7892,9 @@
         <v>691</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="14">
@@ -7924,9 +7910,9 @@
         <v>10</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="14">
@@ -7942,9 +7928,9 @@
         <v>20</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="14">
@@ -7960,9 +7946,9 @@
         <v>692</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="14">
@@ -7978,9 +7964,9 @@
         <v>555</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="17">
@@ -7996,9 +7982,9 @@
         <v>356</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="17">
@@ -8014,9 +8000,9 @@
         <v>542</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="17">
@@ -8032,9 +8018,9 @@
         <v>563</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="17">
@@ -8050,9 +8036,9 @@
         <v>560</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="F29" s="43"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="17">
@@ -8068,9 +8054,9 @@
         <v>10</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F30" s="43"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="17">
@@ -8086,9 +8072,9 @@
         <v>6</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F31" s="43"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="17">
@@ -8104,9 +8090,9 @@
         <v>618</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F32" s="43"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="17">
@@ -8122,9 +8108,9 @@
         <v>691</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F33" s="43"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="17">
@@ -8140,9 +8126,9 @@
         <v>20</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F34" s="43"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="17">
@@ -8158,9 +8144,9 @@
         <v>692</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F35" s="43"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="17">
@@ -8176,9 +8162,9 @@
         <v>555</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F36" s="43"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="17">
@@ -8194,9 +8180,9 @@
         <v>664</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="F37" s="43"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="17">
@@ -8212,8 +8198,9 @@
         <v>356</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F38" s="43"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="17">
@@ -8229,8 +8216,9 @@
         <v>542</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F39" s="43"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="17">
@@ -8246,8 +8234,9 @@
         <v>563</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F40" s="43"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="17">
@@ -8263,8 +8252,9 @@
         <v>560</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F41" s="43"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42" s="17">
@@ -8280,8 +8270,9 @@
         <v>10</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F42" s="43"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43" s="17">
@@ -8297,8 +8288,9 @@
         <v>6</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F43" s="43"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44" s="17">
@@ -8314,8 +8306,9 @@
         <v>691</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F44" s="43"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45" s="17">
@@ -8331,8 +8324,9 @@
         <v>20</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F45" s="43"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1">
       <c r="A46" s="17">
@@ -8348,8 +8342,9 @@
         <v>692</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F46" s="43"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1">
       <c r="A47" s="17">
@@ -8365,8 +8360,9 @@
         <v>555</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F47" s="43"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1">
       <c r="A48" s="17">
@@ -8382,10 +8378,11 @@
         <v>664</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F48" s="43"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
       <c r="A49" s="17">
         <v>48</v>
       </c>
@@ -8399,10 +8396,11 @@
         <v>618</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F49" s="43"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1">
       <c r="A50" s="16">
         <v>50</v>
       </c>
@@ -8416,10 +8414,11 @@
         <v>542</v>
       </c>
       <c r="E50" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F50" s="43"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1">
       <c r="A51" s="16">
         <v>51</v>
       </c>
@@ -8433,10 +8432,11 @@
         <v>563</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F51" s="43"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1">
       <c r="A52" s="16">
         <v>52</v>
       </c>
@@ -8450,10 +8450,11 @@
         <v>356</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F52" s="43"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1">
       <c r="A53" s="16">
         <v>53</v>
       </c>
@@ -8467,10 +8468,11 @@
         <v>560</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F53" s="43"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1">
       <c r="A54" s="16">
         <v>54</v>
       </c>
@@ -8484,10 +8486,11 @@
         <v>664</v>
       </c>
       <c r="E54" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F54" s="43"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1">
       <c r="A55" s="16">
         <v>55</v>
       </c>
@@ -8501,10 +8504,11 @@
         <v>6</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F55" s="43"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1">
       <c r="A56" s="16">
         <v>56</v>
       </c>
@@ -8518,10 +8522,11 @@
         <v>10</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F56" s="43"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1">
       <c r="A57" s="16">
         <v>57</v>
       </c>
@@ -8535,10 +8540,11 @@
         <v>20</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F57" s="43"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1">
       <c r="A58" s="16">
         <v>58</v>
       </c>
@@ -8552,10 +8558,11 @@
         <v>691</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F58" s="43"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1">
       <c r="A59" s="16">
         <v>59</v>
       </c>
@@ -8569,10 +8576,11 @@
         <v>618</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F59" s="43"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1">
       <c r="A60" s="16">
         <v>60</v>
       </c>
@@ -8586,10 +8594,11 @@
         <v>555</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F60" s="43"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1">
       <c r="A61" s="16">
         <v>61</v>
       </c>
@@ -8603,10 +8612,11 @@
         <v>692</v>
       </c>
       <c r="E61" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F61" s="43"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1">
       <c r="A62" s="16">
         <v>62</v>
       </c>
@@ -8620,10 +8630,11 @@
         <v>542</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F62" s="43"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1">
       <c r="A63" s="16">
         <v>63</v>
       </c>
@@ -8637,10 +8648,11 @@
         <v>563</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F63" s="43"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1">
       <c r="A64" s="16">
         <v>64</v>
       </c>
@@ -8654,10 +8666,11 @@
         <v>356</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F64" s="43"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1">
       <c r="A65" s="16">
         <v>65</v>
       </c>
@@ -8671,10 +8684,11 @@
         <v>560</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F65" s="43"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1">
       <c r="A66" s="16">
         <v>66</v>
       </c>
@@ -8688,10 +8702,11 @@
         <v>664</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F66" s="43"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1">
       <c r="A67" s="16">
         <v>67</v>
       </c>
@@ -8705,10 +8720,11 @@
         <v>6</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F67" s="43"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1">
       <c r="A68" s="16">
         <v>68</v>
       </c>
@@ -8722,10 +8738,11 @@
         <v>10</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F68" s="43"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1">
       <c r="A69" s="16">
         <v>69</v>
       </c>
@@ -8739,10 +8756,11 @@
         <v>20</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F69" s="43"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1">
       <c r="A70" s="16">
         <v>70</v>
       </c>
@@ -8756,10 +8774,11 @@
         <v>691</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F70" s="43"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1">
       <c r="A71" s="16">
         <v>71</v>
       </c>
@@ -8773,10 +8792,11 @@
         <v>618</v>
       </c>
       <c r="E71" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F71" s="43"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1">
       <c r="A72" s="16">
         <v>72</v>
       </c>
@@ -8790,10 +8810,11 @@
         <v>555</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F72" s="43"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1">
       <c r="A73" s="16">
         <v>73</v>
       </c>
@@ -8807,10 +8828,11 @@
         <v>692</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="F73" s="43"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1">
       <c r="A74" s="15">
         <v>74</v>
       </c>
@@ -8824,10 +8846,11 @@
         <v>542</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F74" s="43"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1">
       <c r="A75" s="15">
         <v>75</v>
       </c>
@@ -8841,10 +8864,11 @@
         <v>356</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F75" s="43"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1">
       <c r="A76" s="15">
         <v>76</v>
       </c>
@@ -8858,10 +8882,11 @@
         <v>563</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F76" s="43"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1">
       <c r="A77" s="15">
         <v>77</v>
       </c>
@@ -8875,10 +8900,11 @@
         <v>560</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F77" s="43"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1">
       <c r="A78" s="15">
         <v>78</v>
       </c>
@@ -8892,10 +8918,11 @@
         <v>6</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F78" s="43"/>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1">
       <c r="A79" s="15">
         <v>79</v>
       </c>
@@ -8909,10 +8936,11 @@
         <v>555</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F79" s="43"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1">
       <c r="A80" s="15">
         <v>80</v>
       </c>
@@ -8926,10 +8954,11 @@
         <v>664</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F80" s="43"/>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" customHeight="1">
       <c r="A81" s="15">
         <v>81</v>
       </c>
@@ -8943,10 +8972,11 @@
         <v>691</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F81" s="43"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" customHeight="1">
       <c r="A82" s="15">
         <v>82</v>
       </c>
@@ -8960,10 +8990,11 @@
         <v>618</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F82" s="43"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1">
       <c r="A83" s="15">
         <v>83</v>
       </c>
@@ -8977,10 +9008,11 @@
         <v>692</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F83" s="43"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1">
       <c r="A84" s="15">
         <v>84</v>
       </c>
@@ -8994,10 +9026,11 @@
         <v>10</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F84" s="43"/>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" customHeight="1">
       <c r="A85" s="15">
         <v>85</v>
       </c>
@@ -9011,10 +9044,11 @@
         <v>20</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F85" s="43"/>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" customHeight="1">
       <c r="A86" s="15">
         <v>86</v>
       </c>
@@ -9028,10 +9062,11 @@
         <v>356</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F86" s="43"/>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" customHeight="1">
       <c r="A87" s="15">
         <v>87</v>
       </c>
@@ -9045,10 +9080,11 @@
         <v>542</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F87" s="43"/>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1">
       <c r="A88" s="15">
         <v>88</v>
       </c>
@@ -9062,10 +9098,11 @@
         <v>563</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="15.75" customHeight="1">
+        <v>63</v>
+      </c>
+      <c r="F88" s="43"/>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1">
       <c r="A89" s="15">
         <v>89</v>
       </c>
@@ -9079,10 +9116,11 @@
         <v>560</v>
       </c>
       <c r="E89" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F89" s="43"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1">
       <c r="A90" s="15">
         <v>90</v>
       </c>
@@ -9096,10 +9134,11 @@
         <v>664</v>
       </c>
       <c r="E90" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F90" s="43"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1">
       <c r="A91" s="15">
         <v>91</v>
       </c>
@@ -9113,10 +9152,11 @@
         <v>6</v>
       </c>
       <c r="E91" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="15.75" customHeight="1">
+        <v>64</v>
+      </c>
+      <c r="F91" s="43"/>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1">
       <c r="A92" s="15">
         <v>92</v>
       </c>
@@ -9130,10 +9170,11 @@
         <v>691</v>
       </c>
       <c r="E92" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F92" s="43"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1">
       <c r="A93" s="15">
         <v>93</v>
       </c>
@@ -9147,10 +9188,11 @@
         <v>10</v>
       </c>
       <c r="E93" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F93" s="43"/>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1">
       <c r="A94" s="15">
         <v>94</v>
       </c>
@@ -9164,10 +9206,11 @@
         <v>20</v>
       </c>
       <c r="E94" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F94" s="43"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1">
       <c r="A95" s="15">
         <v>95</v>
       </c>
@@ -9181,10 +9224,11 @@
         <v>618</v>
       </c>
       <c r="E95" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15.75" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="F95" s="43"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" customHeight="1">
       <c r="A96" s="15">
         <v>96</v>
       </c>
@@ -9198,8 +9242,9 @@
         <v>692</v>
       </c>
       <c r="E96" s="15" t="s">
-        <v>109</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F96" s="43"/>
     </row>
     <row r="97" spans="1:8" ht="15.75" customHeight="1">
       <c r="A97" s="15">
@@ -9215,425 +9260,450 @@
         <v>555</v>
       </c>
       <c r="E97" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F97" s="43"/>
+    </row>
+    <row r="98" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A98" s="41">
+        <v>98</v>
+      </c>
+      <c r="B98" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C98" s="41">
+        <v>1</v>
+      </c>
+      <c r="D98" s="41">
+        <v>356</v>
+      </c>
+      <c r="E98" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F98" s="43"/>
+    </row>
+    <row r="99" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A99" s="41">
+        <v>99</v>
+      </c>
+      <c r="B99" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C99" s="41">
+        <v>1</v>
+      </c>
+      <c r="D99" s="41">
+        <v>563</v>
+      </c>
+      <c r="E99" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F99" s="43"/>
+    </row>
+    <row r="100" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A100" s="41">
+        <v>100</v>
+      </c>
+      <c r="B100" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C100" s="41">
+        <v>1</v>
+      </c>
+      <c r="D100" s="41">
+        <v>542</v>
+      </c>
+      <c r="E100" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F100" s="43"/>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A101" s="41">
+        <v>101</v>
+      </c>
+      <c r="B101" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C101" s="41">
+        <v>1</v>
+      </c>
+      <c r="D101" s="41">
+        <v>560</v>
+      </c>
+      <c r="E101" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F101" s="43"/>
+    </row>
+    <row r="102" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A102" s="41">
+        <v>102</v>
+      </c>
+      <c r="B102" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C102" s="41">
+        <v>2</v>
+      </c>
+      <c r="D102" s="41">
+        <v>6</v>
+      </c>
+      <c r="E102" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F102" s="43"/>
+    </row>
+    <row r="103" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A103" s="41">
+        <v>103</v>
+      </c>
+      <c r="B103" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C103" s="41">
+        <v>2</v>
+      </c>
+      <c r="D103" s="41">
+        <v>664</v>
+      </c>
+      <c r="E103" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F103" s="43"/>
+    </row>
+    <row r="104" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A104" s="41">
+        <v>104</v>
+      </c>
+      <c r="B104" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C104" s="41">
+        <v>2</v>
+      </c>
+      <c r="D104" s="41">
+        <v>10</v>
+      </c>
+      <c r="E104" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F104" s="43"/>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A105" s="41">
+        <v>105</v>
+      </c>
+      <c r="B105" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C105" s="41">
+        <v>3</v>
+      </c>
+      <c r="D105" s="41">
+        <v>618</v>
+      </c>
+      <c r="E105" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F105" s="43"/>
+    </row>
+    <row r="106" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A106" s="41">
+        <v>106</v>
+      </c>
+      <c r="B106" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C106" s="41">
+        <v>3</v>
+      </c>
+      <c r="D106" s="41">
+        <v>691</v>
+      </c>
+      <c r="E106" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F106" s="43"/>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A107" s="41">
+        <v>107</v>
+      </c>
+      <c r="B107" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C107" s="41">
+        <v>4</v>
+      </c>
+      <c r="D107" s="41">
+        <v>692</v>
+      </c>
+      <c r="E107" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F107" s="43"/>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A108" s="41">
+        <v>108</v>
+      </c>
+      <c r="B108" s="41">
+        <v>7257</v>
+      </c>
+      <c r="C108" s="41">
+        <v>4</v>
+      </c>
+      <c r="D108" s="41">
+        <v>555</v>
+      </c>
+      <c r="E108" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F108" s="43"/>
+    </row>
+    <row r="109" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A109" s="41">
         <v>109</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A98" s="42">
-        <v>98</v>
-      </c>
-      <c r="B98" s="42">
+      <c r="B109" s="41">
         <v>7257</v>
       </c>
-      <c r="C98" s="42">
+      <c r="C109" s="41">
+        <v>4</v>
+      </c>
+      <c r="D109" s="41">
+        <v>20</v>
+      </c>
+      <c r="E109" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F109" s="43"/>
+    </row>
+    <row r="110" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A110" s="41">
+        <v>110</v>
+      </c>
+      <c r="B110" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C110" s="41">
         <v>1</v>
       </c>
-      <c r="D98" s="42">
+      <c r="D110" s="41">
         <v>356</v>
       </c>
-      <c r="E98" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A99" s="42">
-        <v>99</v>
-      </c>
-      <c r="B99" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C99" s="42">
+      <c r="E110" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F110" s="43"/>
+      <c r="H110" s="42"/>
+    </row>
+    <row r="111" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A111" s="41">
+        <v>111</v>
+      </c>
+      <c r="B111" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C111" s="41">
         <v>1</v>
       </c>
-      <c r="D99" s="42">
+      <c r="D111" s="41">
         <v>563</v>
       </c>
-      <c r="E99" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A100" s="42">
-        <v>100</v>
-      </c>
-      <c r="B100" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C100" s="42">
+      <c r="E111" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F111" s="43"/>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A112" s="41">
+        <v>112</v>
+      </c>
+      <c r="B112" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C112" s="41">
         <v>1</v>
       </c>
-      <c r="D100" s="42">
+      <c r="D112" s="41">
         <v>542</v>
       </c>
-      <c r="E100" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A101" s="42">
-        <v>101</v>
-      </c>
-      <c r="B101" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C101" s="42">
+      <c r="E112" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F112" s="43"/>
+    </row>
+    <row r="113" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A113" s="41">
+        <v>113</v>
+      </c>
+      <c r="B113" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C113" s="41">
         <v>1</v>
       </c>
-      <c r="D101" s="42">
+      <c r="D113" s="41">
         <v>560</v>
       </c>
-      <c r="E101" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A102" s="42">
-        <v>102</v>
-      </c>
-      <c r="B102" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C102" s="42">
+      <c r="E113" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F113" s="43"/>
+    </row>
+    <row r="114" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A114" s="41">
+        <v>114</v>
+      </c>
+      <c r="B114" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C114" s="41">
         <v>2</v>
       </c>
-      <c r="D102" s="42">
+      <c r="D114" s="41">
         <v>6</v>
       </c>
-      <c r="E102" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A103" s="42">
-        <v>103</v>
-      </c>
-      <c r="B103" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C103" s="42">
+      <c r="E114" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F114" s="43"/>
+    </row>
+    <row r="115" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A115" s="41">
+        <v>115</v>
+      </c>
+      <c r="B115" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C115" s="41">
         <v>2</v>
       </c>
-      <c r="D103" s="42">
+      <c r="D115" s="41">
         <v>664</v>
       </c>
-      <c r="E103" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A104" s="42">
-        <v>104</v>
-      </c>
-      <c r="B104" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C104" s="42">
+      <c r="E115" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F115" s="43"/>
+    </row>
+    <row r="116" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A116" s="41">
+        <v>116</v>
+      </c>
+      <c r="B116" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C116" s="41">
         <v>2</v>
       </c>
-      <c r="D104" s="42">
+      <c r="D116" s="41">
         <v>10</v>
       </c>
-      <c r="E104" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A105" s="42">
-        <v>105</v>
-      </c>
-      <c r="B105" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C105" s="42">
+      <c r="E116" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F116" s="43"/>
+    </row>
+    <row r="117" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A117" s="41">
+        <v>117</v>
+      </c>
+      <c r="B117" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C117" s="41">
         <v>3</v>
       </c>
-      <c r="D105" s="42">
+      <c r="D117" s="41">
+        <v>691</v>
+      </c>
+      <c r="E117" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F117" s="43"/>
+    </row>
+    <row r="118" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A118" s="41">
+        <v>118</v>
+      </c>
+      <c r="B118" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C118" s="41">
+        <v>3</v>
+      </c>
+      <c r="D118" s="41">
+        <v>20</v>
+      </c>
+      <c r="E118" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F118" s="43"/>
+    </row>
+    <row r="119" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A119" s="41">
+        <v>119</v>
+      </c>
+      <c r="B119" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C119" s="41">
+        <v>4</v>
+      </c>
+      <c r="D119" s="41">
+        <v>692</v>
+      </c>
+      <c r="E119" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F119" s="43"/>
+    </row>
+    <row r="120" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A120" s="41">
+        <v>120</v>
+      </c>
+      <c r="B120" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C120" s="41">
+        <v>4</v>
+      </c>
+      <c r="D120" s="41">
+        <v>555</v>
+      </c>
+      <c r="E120" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F120" s="43"/>
+    </row>
+    <row r="121" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A121" s="41">
+        <v>121</v>
+      </c>
+      <c r="B121" s="41">
+        <v>7258</v>
+      </c>
+      <c r="C121" s="41">
+        <v>5</v>
+      </c>
+      <c r="D121" s="41">
         <v>618</v>
       </c>
-      <c r="E105" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A106" s="42">
-        <v>106</v>
-      </c>
-      <c r="B106" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C106" s="42">
-        <v>3</v>
-      </c>
-      <c r="D106" s="42">
-        <v>691</v>
-      </c>
-      <c r="E106" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A107" s="42">
-        <v>107</v>
-      </c>
-      <c r="B107" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C107" s="42">
-        <v>4</v>
-      </c>
-      <c r="D107" s="42">
-        <v>692</v>
-      </c>
-      <c r="E107" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A108" s="42">
-        <v>108</v>
-      </c>
-      <c r="B108" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C108" s="42">
-        <v>4</v>
-      </c>
-      <c r="D108" s="42">
-        <v>555</v>
-      </c>
-      <c r="E108" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A109" s="42">
-        <v>109</v>
-      </c>
-      <c r="B109" s="42">
-        <v>7257</v>
-      </c>
-      <c r="C109" s="42">
-        <v>4</v>
-      </c>
-      <c r="D109" s="42">
-        <v>20</v>
-      </c>
-      <c r="E109" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A110" s="42">
-        <v>110</v>
-      </c>
-      <c r="B110" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C110" s="42">
-        <v>1</v>
-      </c>
-      <c r="D110" s="42">
-        <v>356</v>
-      </c>
-      <c r="E110" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="H110" s="43"/>
-    </row>
-    <row r="111" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A111" s="42">
-        <v>111</v>
-      </c>
-      <c r="B111" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C111" s="42">
-        <v>1</v>
-      </c>
-      <c r="D111" s="42">
-        <v>563</v>
-      </c>
-      <c r="E111" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A112" s="42">
-        <v>112</v>
-      </c>
-      <c r="B112" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C112" s="42">
-        <v>1</v>
-      </c>
-      <c r="D112" s="42">
-        <v>542</v>
-      </c>
-      <c r="E112" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A113" s="42">
-        <v>113</v>
-      </c>
-      <c r="B113" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C113" s="42">
-        <v>1</v>
-      </c>
-      <c r="D113" s="42">
-        <v>560</v>
-      </c>
-      <c r="E113" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A114" s="42">
-        <v>114</v>
-      </c>
-      <c r="B114" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C114" s="42">
-        <v>2</v>
-      </c>
-      <c r="D114" s="42">
-        <v>6</v>
-      </c>
-      <c r="E114" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A115" s="42">
-        <v>115</v>
-      </c>
-      <c r="B115" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C115" s="42">
-        <v>2</v>
-      </c>
-      <c r="D115" s="42">
-        <v>664</v>
-      </c>
-      <c r="E115" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A116" s="42">
-        <v>116</v>
-      </c>
-      <c r="B116" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C116" s="42">
-        <v>2</v>
-      </c>
-      <c r="D116" s="42">
-        <v>10</v>
-      </c>
-      <c r="E116" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A117" s="42">
-        <v>117</v>
-      </c>
-      <c r="B117" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C117" s="42">
-        <v>3</v>
-      </c>
-      <c r="D117" s="42">
-        <v>691</v>
-      </c>
-      <c r="E117" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A118" s="42">
-        <v>118</v>
-      </c>
-      <c r="B118" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C118" s="42">
-        <v>3</v>
-      </c>
-      <c r="D118" s="42">
-        <v>20</v>
-      </c>
-      <c r="E118" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A119" s="42">
-        <v>119</v>
-      </c>
-      <c r="B119" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C119" s="42">
-        <v>4</v>
-      </c>
-      <c r="D119" s="42">
-        <v>692</v>
-      </c>
-      <c r="E119" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A120" s="42">
-        <v>120</v>
-      </c>
-      <c r="B120" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C120" s="42">
-        <v>4</v>
-      </c>
-      <c r="D120" s="42">
-        <v>555</v>
-      </c>
-      <c r="E120" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A121" s="42">
-        <v>121</v>
-      </c>
-      <c r="B121" s="42">
-        <v>7258</v>
-      </c>
-      <c r="C121" s="42">
-        <v>5</v>
-      </c>
-      <c r="D121" s="42">
-        <v>618</v>
-      </c>
-      <c r="E121" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="123" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="124" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="125" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="126" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="127" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="128" spans="1:5" ht="15.75" customHeight="1"/>
+      <c r="E121" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="F121" s="43"/>
+    </row>
+    <row r="122" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="123" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="124" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="125" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="126" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="127" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="128" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="129" ht="15.75" customHeight="1"/>
     <row r="130" ht="15.75" customHeight="1"/>
     <row r="131" ht="15.75" customHeight="1"/>
@@ -10534,19 +10604,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -10560,10 +10630,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10577,10 +10647,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10594,10 +10664,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10611,10 +10681,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
@@ -10628,10 +10698,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
@@ -10645,10 +10715,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
@@ -10662,10 +10732,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
@@ -10679,10 +10749,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10696,10 +10766,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10713,10 +10783,10 @@
         <v>2</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10730,10 +10800,10 @@
         <v>3</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10747,10 +10817,10 @@
         <v>4</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10764,10 +10834,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1">
@@ -10781,10 +10851,10 @@
         <v>2</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1">
@@ -10798,10 +10868,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
@@ -10815,10 +10885,10 @@
         <v>4</v>
       </c>
       <c r="D17" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
@@ -10832,10 +10902,10 @@
         <v>5</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
@@ -10849,10 +10919,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
@@ -10866,10 +10936,10 @@
         <v>2</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
@@ -10883,10 +10953,10 @@
         <v>3</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
@@ -10900,10 +10970,10 @@
         <v>4</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -10917,10 +10987,10 @@
         <v>5</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -10934,10 +11004,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
@@ -10951,10 +11021,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
@@ -10968,10 +11038,10 @@
         <v>3</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
@@ -10985,10 +11055,10 @@
         <v>4</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
@@ -11002,10 +11072,10 @@
         <v>5</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
@@ -11019,10 +11089,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
@@ -11036,10 +11106,10 @@
         <v>2</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
@@ -11053,10 +11123,10 @@
         <v>3</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
@@ -11070,10 +11140,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
@@ -11087,10 +11157,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
@@ -11104,10 +11174,10 @@
         <v>2</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
@@ -11121,10 +11191,10 @@
         <v>3</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
@@ -11138,10 +11208,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
@@ -11155,10 +11225,10 @@
         <v>5</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
@@ -11172,10 +11242,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
@@ -11189,10 +11259,10 @@
         <v>2</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
@@ -11206,10 +11276,10 @@
         <v>3</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1">
@@ -11223,10 +11293,10 @@
         <v>4</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
@@ -11240,10 +11310,10 @@
         <v>1</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
@@ -11257,10 +11327,10 @@
         <v>2</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1">
@@ -11274,10 +11344,10 @@
         <v>3</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1">
@@ -11291,10 +11361,10 @@
         <v>4</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1">
@@ -11308,10 +11378,10 @@
         <v>5</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>